<commit_message>
Dyanmic list and dependent, autoformatter, slicers, advance filtering
</commit_message>
<xml_diff>
--- a/11. Dynamic Dropdown LIst/dynamic_list.xlsx
+++ b/11. Dynamic Dropdown LIst/dynamic_list.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advance_Excel_BI\11. Dynamic Dropdown LIst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F880E0D-E6BD-47A3-BC14-A8158AD8A49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23177498-8DF0-4221-847F-6ADDCE348501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DFBDDC44-5B26-4933-9FE5-39F5FC447B3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dynamic_List_or_Dependent _Drop" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Canada">Sheet1!$I$7:$I$9</definedName>
-    <definedName name="China">Sheet1!$H$7:$H$9</definedName>
-    <definedName name="Cities">Sheet1!$F$6:$I$6</definedName>
-    <definedName name="Countries" localSheetId="0">Sheet1!$F$6:$I$6</definedName>
-    <definedName name="Country">Sheet1!$F$6:$I$11</definedName>
-    <definedName name="India">Sheet1!$F$7:$F$11</definedName>
-    <definedName name="Malaysia">Sheet1!$G$7:$G$9</definedName>
+    <definedName name="Australia">'Dynamic_List_or_Dependent _Drop'!$K$9</definedName>
+    <definedName name="Canada">'Dynamic_List_or_Dependent _Drop'!$J$9:$J$11</definedName>
+    <definedName name="China">'Dynamic_List_or_Dependent _Drop'!$I$9:$I$11</definedName>
+    <definedName name="India">'Dynamic_List_or_Dependent _Drop'!$G$9:$G$13</definedName>
+    <definedName name="Malaysia">'Dynamic_List_or_Dependent _Drop'!$H$9:$H$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>India</t>
   </si>
@@ -120,6 +118,15 @@
       </rPr>
       <t>Prequisite:- Name Range is required for dependent dropdown list.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> =INDIRECT()</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Sydney</t>
   </si>
 </sst>
 </file>
@@ -505,170 +512,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EDE40A-0F65-4963-A264-306376672C98}">
-  <dimension ref="A1:P15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D145778-29CE-4502-B2CF-13A1A82FD269}">
+  <dimension ref="A2:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F6" s="1" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F7" t="s">
+      <c r="K8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I9" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F8" t="s">
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I10" t="s">
         <v>13</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
+      <c r="P10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H11" t="s">
         <v>11</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I11" t="s">
         <v>14</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F11" t="s">
+      <c r="P12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G14" t="s">
+      <c r="O15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" t="s">
-        <v>18</v>
-      </c>
-      <c r="P14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>5</v>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E5"/>
+    <mergeCell ref="A2:E6"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15 F6:I6 I15" xr:uid="{75CE89D9-919D-4A9D-A8D7-5C6E8DA32DDD}">
-      <formula1>$F$6:$I$6</formula1>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N16" xr:uid="{6F405A17-0E21-45D0-B000-DAA268EF3528}">
+      <formula1>$G$8:$J$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15" xr:uid="{6917C64A-0B15-4254-99F6-D2D7DA87BE73}">
-      <formula1>INDIRECT($F$15)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O16" xr:uid="{A50204B0-4349-4AA3-8F2C-732589F156FF}">
+      <formula1>INDIRECT($N$16)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15" xr:uid="{5B0D99B1-A266-4615-88FE-179B61EEF876}">
-      <formula1>INDIRECT($I$15)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P10:P51" xr:uid="{201EC266-E318-4FA2-8EC0-2E68933BF453}">
+      <formula1>$G$8:$K$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q12:Q51" xr:uid="{9A054DB6-FF0A-442C-9647-A208F394FDAE}">
+      <formula1>INDIRECT($P$10)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q10:Q11" xr:uid="{8279EBAA-2AD3-424B-BECB-1352A5A3BA54}">
+      <formula1>INDIRECT($P10)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>